<commit_message>
feat(lokasi): implement server-side processing for Cabang table with enhanced filtering and ordering
</commit_message>
<xml_diff>
--- a/dashboard/assets/template/template_anggota_cs.xlsx
+++ b/dashboard/assets/template/template_anggota_cs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Husni Aditya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laragon\www\ciptasejati\dashboard\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,9 +30,6 @@
     <t>ANGGOTA_ID</t>
   </si>
   <si>
-    <t>003.003.2008.008</t>
-  </si>
-  <si>
     <t>Ranting Mentaya</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>Koordinator</t>
-  </si>
-  <si>
-    <t>003.003.2010.022</t>
   </si>
   <si>
     <t>Ranting Mentaya-II</t>
@@ -106,9 +100,6 @@
     <t>Tidak Aktif</t>
   </si>
   <si>
-    <t>001.003.003</t>
-  </si>
-  <si>
     <t>CABANG_ID</t>
   </si>
   <si>
@@ -158,6 +149,15 @@
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>03.02.2013.00125</t>
+  </si>
+  <si>
+    <t>03.02.2024.00270</t>
+  </si>
+  <si>
+    <t>01.03.02</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -511,152 +513,152 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
       </c>
       <c r="L2" s="1">
         <v>30272</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" s="1">
         <v>39745</v>
       </c>
       <c r="Q2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
       </c>
       <c r="L3" s="1">
         <v>32735</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O3" s="1">
         <v>40358</v>
@@ -665,10 +667,10 @@
         <v>43492</v>
       </c>
       <c r="Q3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>